<commit_message>
Fix fetch URLs for live deployment
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,32 +417,12 @@
     </row>
     <row r="3">
       <c r="B3" t="str">
-        <v>87346</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>malik0580281@gmail.com</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="str">
-        <v>87346</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>amazinglepords.20.10@gmail.com</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="str">
-        <v>87346</v>
+        <v>zaz</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>